<commit_message>
Add data for results Fig1, Fig3, FigS31, and supp tables 4,5
</commit_message>
<xml_diff>
--- a/script_overview.xlsx
+++ b/script_overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pb637\Documents\Yale Courses\Research\Final Paper\resstock_projections\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Documents\projects\Yale\resstock_projections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530884D4-67E4-4606-8F44-5E668F1119AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCE9A4E-E999-4ED2-8F06-3885BC0C7C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="projection" sheetId="1" r:id="rId1"/>
@@ -711,12 +711,6 @@
     <t>none, just create some figures</t>
   </si>
   <si>
-    <t>Supplementary_results/EI_seg_base.csv</t>
-  </si>
-  <si>
-    <t>Supplementary_results/EI.csv</t>
-  </si>
-  <si>
     <t>tot_GHG_2005_2020.R</t>
   </si>
   <si>
@@ -768,15 +762,6 @@
     <t>All res* files in Final_results/</t>
   </si>
   <si>
-    <t>Final_results/GHGall_new.RData</t>
-  </si>
-  <si>
-    <t>Final_results/GHG_Source_new.RData</t>
-  </si>
-  <si>
-    <t>Figure data in csv or sometimes .RData files</t>
-  </si>
-  <si>
     <t>Many figure files which need manually saved</t>
   </si>
   <si>
@@ -796,6 +781,21 @@
   </si>
   <si>
     <t>RS_results_all</t>
+  </si>
+  <si>
+    <t>Final_results/supp_Tab5.csv</t>
+  </si>
+  <si>
+    <t>Final_results/supp_Tab4.csv</t>
+  </si>
+  <si>
+    <t>Final_results/GHGall.RData</t>
+  </si>
+  <si>
+    <t>Final_results/GHG_Source.RData</t>
+  </si>
+  <si>
+    <t>Figure data in csv files, in Figure_Results_Data, for Fig1, Fig3, FigS31</t>
   </si>
 </sst>
 </file>
@@ -1115,18 +1115,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.53125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>19</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
         <v>20</v>
       </c>
@@ -1179,12 +1179,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>19</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
         <v>20</v>
       </c>
@@ -1217,12 +1217,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>19</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>20</v>
       </c>
@@ -1255,12 +1255,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>4</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>8</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>9</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>5</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
         <v>32</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>33</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>34</v>
       </c>
@@ -1340,22 +1340,22 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>6</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>32</v>
       </c>
@@ -1383,12 +1383,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E26" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>7</v>
       </c>
@@ -1408,22 +1408,22 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E29" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>8</v>
       </c>
@@ -1434,16 +1434,16 @@
         <v>51</v>
       </c>
       <c r="D31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E31" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F31" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>9</v>
       </c>
@@ -1463,12 +1463,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>10</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D35" t="s">
         <v>62</v>
       </c>
@@ -1493,12 +1493,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>11</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
         <v>69</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
         <v>70</v>
       </c>
@@ -1534,37 +1534,37 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D43" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D45" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>12</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>13</v>
       </c>
@@ -1604,27 +1604,27 @@
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D48" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D49" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D50" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D51" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>14</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D53" t="s">
         <v>94</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D54" t="s">
         <v>95</v>
       </c>
@@ -1660,12 +1660,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D55" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D56" t="s">
         <v>97</v>
       </c>
@@ -1679,17 +1679,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B77A6A4-E700-4667-BE58-A58B09F8FC11}">
   <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L100" sqref="L100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O108" sqref="O108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D2" t="s">
         <v>173</v>
@@ -1729,7 +1729,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>174</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
         <v>175</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>176</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
         <v>177</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>178</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
         <v>179</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
         <v>180</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>181</v>
       </c>
@@ -1793,107 +1793,107 @@
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>101</v>
       </c>
       <c r="C32" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D32" t="s">
         <v>102</v>
@@ -1910,7 +1910,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
         <v>103</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
         <v>104</v>
       </c>
@@ -1926,32 +1926,32 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E35" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E36" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E37" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E38" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="E37" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="E38" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E39" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>3</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>101</v>
       </c>
       <c r="C41" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D41" t="s">
         <v>111</v>
@@ -1971,7 +1971,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
         <v>68</v>
       </c>
@@ -1979,22 +1979,22 @@
         <v>166</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D43" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D45" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>4</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>101</v>
       </c>
       <c r="C47" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D47" t="s">
         <v>77</v>
@@ -2014,7 +2014,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D48" t="s">
         <v>115</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="49" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D49" t="s">
         <v>116</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="50" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="50" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D50" t="s">
         <v>117</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="51" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="51" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D51" t="s">
         <v>118</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="52" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D52" t="s">
         <v>119</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="53" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="53" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D53" t="s">
         <v>120</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="54" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="54" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D54" t="s">
         <v>121</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="55" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="55" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D55" t="s">
         <v>102</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="56" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="56" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D56" t="s">
         <v>103</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="57" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="57" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D57" t="s">
         <v>104</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="58" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="58" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D58" t="s">
         <v>122</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="59" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="59" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D59" t="s">
         <v>123</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="60" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D60" t="s">
         <v>124</v>
       </c>
@@ -2118,7 +2118,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="61" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="61" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D61" t="s">
         <v>125</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="62" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="62" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D62" t="s">
         <v>126</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="63" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="63" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D63" t="s">
         <v>127</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="64" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="64" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D64" t="s">
         <v>128</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D65" t="s">
         <v>129</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D66" t="s">
         <v>130</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D67" t="s">
         <v>131</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D68" t="s">
         <v>132</v>
       </c>
@@ -2182,57 +2182,57 @@
         <v>155</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E69" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E70" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E71" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E72" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E73" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E74" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E75" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E76" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E77" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E78" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>5</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>101</v>
       </c>
       <c r="C80" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D80" t="s">
         <v>205</v>
@@ -2252,77 +2252,77 @@
         <v>214</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D81" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D82" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D83" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D84" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D85" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D86" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D87" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D88" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D89" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D90" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D91" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D92" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D93" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D94" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>6</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D97" t="s">
         <v>103</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D98" t="s">
         <v>104</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D99" t="s">
         <v>220</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D100" t="s">
         <v>221</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>7</v>
       </c>
@@ -2379,19 +2379,19 @@
         <v>101</v>
       </c>
       <c r="C102" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D102" t="s">
         <v>205</v>
       </c>
       <c r="E102" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F102" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>8</v>
       </c>
@@ -2399,47 +2399,47 @@
         <v>101</v>
       </c>
       <c r="C104" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D104" t="s">
         <v>205</v>
       </c>
       <c r="E104" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D105" t="s">
+        <v>240</v>
+      </c>
+      <c r="E105" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D106" t="s">
+        <v>241</v>
+      </c>
+      <c r="E106" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E107" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E108" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E109" t="s">
         <v>242</v>
       </c>
-      <c r="E105" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="D106" t="s">
-        <v>243</v>
-      </c>
-      <c r="E106" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="E107" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="E108" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="E109" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>9</v>
       </c>
@@ -2447,44 +2447,44 @@
         <v>101</v>
       </c>
       <c r="C111" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D111" t="s">
         <v>213</v>
       </c>
       <c r="E111" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F111" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D112" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.45">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D113" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D114" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D115" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D116" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>10</v>
       </c>
@@ -2492,16 +2492,16 @@
         <v>101</v>
       </c>
       <c r="C118" t="s">
+        <v>228</v>
+      </c>
+      <c r="D118" t="s">
+        <v>229</v>
+      </c>
+      <c r="E118" t="s">
         <v>230</v>
       </c>
-      <c r="D118" t="s">
-        <v>231</v>
-      </c>
-      <c r="E118" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>11</v>
       </c>
@@ -2518,22 +2518,22 @@
         <v>224</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D121" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D122" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D123" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>12</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D126" t="s">
         <v>204</v>
       </c>

</xml_diff>

<commit_message>
Add SI Tables, add base_weights_NC and rencombs to Intermediate_results
</commit_message>
<xml_diff>
--- a/script_overview.xlsx
+++ b/script_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Documents\projects\Yale\resstock_projections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCE9A4E-E999-4ED2-8F06-3885BC0C7C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15D0BFC-2A7A-4063-9D77-D09840BF3DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="projection" sheetId="1" r:id="rId1"/>
@@ -159,9 +159,6 @@
     <t>Calculate projected decay of housing stock by county, vintage/cohort, and house type (3) for each five years 2020-2060</t>
   </si>
   <si>
-    <t>County_Scenario_SM_Results.RData</t>
-  </si>
-  <si>
     <t>decayFactors.RData</t>
   </si>
   <si>
@@ -174,9 +171,6 @@
     <t>Define more efficient windows, infiltration, insulation, AC, in new homes built after 2020, depending on the state and projected adoption of energy efficiency codes/standards</t>
   </si>
   <si>
-    <t>All of the future construction files for each housing stock/new housing characteristics scenario in scen_bscsv</t>
-  </si>
-  <si>
     <t>All of the files in scen_bscsv_adj which include the adjustments made in this script</t>
   </si>
   <si>
@@ -796,6 +790,12 @@
   </si>
   <si>
     <t>Figure data in csv files, in Figure_Results_Data, for Fig1, Fig3, FigS31</t>
+  </si>
+  <si>
+    <t>County_Scenario_SM_Results.Rdata. For access email peter.berrill@aya.yale.edu</t>
+  </si>
+  <si>
+    <t>All of the future construction files for each housing stock/new housing characteristics scenario in scen_bscsv. For access email peter.berrill@aya.yale.edu</t>
   </si>
 </sst>
 </file>
@@ -1115,9 +1115,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1307,10 +1307,10 @@
         <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F17" t="s">
         <v>31</v>
@@ -1366,10 +1366,10 @@
         <v>39</v>
       </c>
       <c r="D24" t="s">
+        <v>252</v>
+      </c>
+      <c r="E24" t="s">
         <v>41</v>
-      </c>
-      <c r="E24" t="s">
-        <v>42</v>
       </c>
       <c r="F24" t="s">
         <v>40</v>
@@ -1385,7 +1385,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1396,31 +1396,31 @@
         <v>5</v>
       </c>
       <c r="C27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" t="s">
+        <v>253</v>
+      </c>
+      <c r="E27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" t="s">
         <v>44</v>
-      </c>
-      <c r="D27" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" t="s">
-        <v>47</v>
-      </c>
-      <c r="F27" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E28" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E29" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1431,16 +1431,16 @@
         <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D31" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E31" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F31" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1451,21 +1451,21 @@
         <v>5</v>
       </c>
       <c r="C32" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" t="s">
         <v>55</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>57</v>
       </c>
-      <c r="E32" t="s">
-        <v>59</v>
-      </c>
       <c r="F32" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1476,26 +1476,26 @@
         <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D34" t="s">
+        <v>59</v>
+      </c>
+      <c r="F34" t="s">
         <v>61</v>
-      </c>
-      <c r="F34" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D35" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" t="s">
         <v>62</v>
-      </c>
-      <c r="E35" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1506,62 +1506,62 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" t="s">
+        <v>66</v>
+      </c>
+      <c r="E37" t="s">
+        <v>75</v>
+      </c>
+      <c r="F37" t="s">
         <v>65</v>
-      </c>
-      <c r="D37" t="s">
-        <v>68</v>
-      </c>
-      <c r="E37" t="s">
-        <v>77</v>
-      </c>
-      <c r="F37" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E38" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E39" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D45" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1572,16 +1572,16 @@
         <v>5</v>
       </c>
       <c r="C46" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" t="s">
+        <v>79</v>
+      </c>
+      <c r="E46" t="s">
         <v>80</v>
       </c>
-      <c r="D46" t="s">
+      <c r="F46" t="s">
         <v>81</v>
-      </c>
-      <c r="E46" t="s">
-        <v>82</v>
-      </c>
-      <c r="F46" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1592,26 +1592,26 @@
         <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D47" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E47" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F47" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D48" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D49" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1621,7 +1621,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D51" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1632,42 +1632,42 @@
         <v>5</v>
       </c>
       <c r="C52" t="s">
+        <v>89</v>
+      </c>
+      <c r="D52" t="s">
         <v>91</v>
       </c>
-      <c r="D52" t="s">
-        <v>93</v>
-      </c>
       <c r="E52" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F52" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D53" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E53" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D54" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E54" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D55" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D56" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1679,9 +1679,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B77A6A4-E700-4667-BE58-A58B09F8FC11}">
   <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O108" sqref="O108"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1714,183 +1714,183 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1898,57 +1898,57 @@
         <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C32" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D32" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E32" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E34" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E35" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E36" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E37" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E38" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E39" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1956,42 +1956,42 @@
         <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C41" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D41" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E41" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E42" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D43" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D45" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1999,237 +1999,237 @@
         <v>4</v>
       </c>
       <c r="B47" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C47" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D47" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E47" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F47" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D48" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E48" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="49" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D49" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E49" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="50" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D50" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E50" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D51" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E51" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D52" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E52" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D53" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E53" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D54" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E54" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D55" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E55" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="56" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D56" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E56" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="57" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D57" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E57" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D58" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E58" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="59" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D59" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E59" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D60" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E60" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="61" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D61" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E61" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="62" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D62" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E62" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="63" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D63" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E63" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="64" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D64" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E64" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D65" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E65" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D66" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E66" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D67" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E67" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D68" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E68" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E69" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E70" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E71" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E72" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E73" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E74" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E75" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E76" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E77" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E78" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2237,89 +2237,89 @@
         <v>5</v>
       </c>
       <c r="B80" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C80" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D80" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E80" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F80" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D81" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D82" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D83" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D84" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D85" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D86" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D87" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D88" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D89" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D90" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D91" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D92" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D93" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D94" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
@@ -2327,48 +2327,48 @@
         <v>6</v>
       </c>
       <c r="B96" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C96" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D96" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E96" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D97" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E97" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D98" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E98" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D99" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E99" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D100" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E100" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2376,19 +2376,19 @@
         <v>7</v>
       </c>
       <c r="B102" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C102" t="s">
+        <v>223</v>
+      </c>
+      <c r="D102" t="s">
+        <v>203</v>
+      </c>
+      <c r="E102" t="s">
+        <v>224</v>
+      </c>
+      <c r="F102" t="s">
         <v>225</v>
-      </c>
-      <c r="D102" t="s">
-        <v>205</v>
-      </c>
-      <c r="E102" t="s">
-        <v>226</v>
-      </c>
-      <c r="F102" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -2396,47 +2396,47 @@
         <v>8</v>
       </c>
       <c r="B104" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C104" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D104" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E104" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D105" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E105" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D106" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E106" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E107" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E108" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E109" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -2444,44 +2444,44 @@
         <v>9</v>
       </c>
       <c r="B111" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C111" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D111" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E111" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F111" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D112" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D113" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D114" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D115" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D116" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
@@ -2489,16 +2489,16 @@
         <v>10</v>
       </c>
       <c r="B118" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C118" t="s">
+        <v>226</v>
+      </c>
+      <c r="D118" t="s">
+        <v>227</v>
+      </c>
+      <c r="E118" t="s">
         <v>228</v>
-      </c>
-      <c r="D118" t="s">
-        <v>229</v>
-      </c>
-      <c r="E118" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
@@ -2506,31 +2506,31 @@
         <v>11</v>
       </c>
       <c r="B120" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C120" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D120" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E120" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D121" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D122" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D123" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
@@ -2538,18 +2538,18 @@
         <v>12</v>
       </c>
       <c r="B125" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C125" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D125" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D126" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update results_scripts files and add small files in *_results and Figure_Results_Data folders
</commit_message>
<xml_diff>
--- a/script_overview.xlsx
+++ b/script_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Documents\projects\Yale\resstock_projections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15D0BFC-2A7A-4063-9D77-D09840BF3DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917130FD-8833-47A2-B185-4F7EAAF5DC38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="projection" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="260">
   <si>
     <t>Folder</t>
   </si>
@@ -675,9 +675,6 @@
     <t>Assess GHG reductions from scenarios, for particular combinations, geographical and housing stock based. Make some linear models to help assess the main influences on emission reductions in different scenarios</t>
   </si>
   <si>
-    <t>ren_ass_strategy</t>
-  </si>
-  <si>
     <t>Final_results/ren_strat_comp.RData</t>
   </si>
   <si>
@@ -690,15 +687,6 @@
     <t>Final_results/ren_NPV.RData</t>
   </si>
   <si>
-    <t>ExtData/CBA_prices/MT.csv</t>
-  </si>
-  <si>
-    <t>ExtData/CBA_prices/ESC.csv</t>
-  </si>
-  <si>
-    <t>Final_results/ren_div_sum.csv</t>
-  </si>
-  <si>
     <t>develop_newHP</t>
   </si>
   <si>
@@ -796,6 +784,36 @@
   </si>
   <si>
     <t>All of the future construction files for each housing stock/new housing characteristics scenario in scen_bscsv. For access email peter.berrill@aya.yale.edu</t>
+  </si>
+  <si>
+    <t>Calculate % reductions in final energy consumption from different renovation families in each renovation scenario, for SI Tables S6 and S7. Calculate number of renovations by type in each ren scenario</t>
+  </si>
+  <si>
+    <t>Figure_Results_Data/GHG_scen_comp_StateCty.xlsx</t>
+  </si>
+  <si>
+    <t>ren_assess_strategy</t>
+  </si>
+  <si>
+    <t>Final_results/ren_NPV.xlsx</t>
+  </si>
+  <si>
+    <t>Test the benefits of individual renovation strategies in different scenarios. Make environmental-economic cost-benefit analysis of renovation strategies</t>
+  </si>
+  <si>
+    <t>Final_results/supp_Tab3.csv</t>
+  </si>
+  <si>
+    <t>ExtData/CBA_prices/* fuel prices by division</t>
+  </si>
+  <si>
+    <t>ExtData/CapExHeat.csv</t>
+  </si>
+  <si>
+    <t>ExtData/CapExDHW.csv</t>
+  </si>
+  <si>
+    <t>ExtData/CapExIns.csv</t>
   </si>
 </sst>
 </file>
@@ -1115,9 +1133,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1366,7 +1384,7 @@
         <v>39</v>
       </c>
       <c r="D24" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E24" t="s">
         <v>41</v>
@@ -1399,7 +1417,7 @@
         <v>43</v>
       </c>
       <c r="D27" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E27" t="s">
         <v>45</v>
@@ -1434,10 +1452,10 @@
         <v>49</v>
       </c>
       <c r="D31" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E31" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F31" t="s">
         <v>50</v>
@@ -1677,16 +1695,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B77A6A4-E700-4667-BE58-A58B09F8FC11}">
-  <dimension ref="A1:F126"/>
+  <dimension ref="A1:F128"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.109375" customWidth="1"/>
+    <col min="5" max="5" width="43.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -1717,7 +1737,7 @@
         <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D2" t="s">
         <v>171</v>
@@ -1823,77 +1843,77 @@
         <v>185</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2</v>
       </c>
@@ -1901,13 +1921,16 @@
         <v>99</v>
       </c>
       <c r="C32" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D32" t="s">
         <v>100</v>
       </c>
       <c r="E32" t="s">
         <v>103</v>
+      </c>
+      <c r="F32" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1933,17 +1956,17 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E36" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E37" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E38" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1959,7 +1982,7 @@
         <v>99</v>
       </c>
       <c r="C41" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D41" t="s">
         <v>109</v>
@@ -2002,7 +2025,7 @@
         <v>99</v>
       </c>
       <c r="C47" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D47" t="s">
         <v>75</v>
@@ -2240,7 +2263,7 @@
         <v>99</v>
       </c>
       <c r="C80" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D80" t="s">
         <v>203</v>
@@ -2252,77 +2275,80 @@
         <v>212</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D81" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E81" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D82" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D83" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D84" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D85" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D86" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D87" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D88" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D89" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D90" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D91" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D92" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D93" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D94" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>6</v>
       </c>
@@ -2330,13 +2356,16 @@
         <v>99</v>
       </c>
       <c r="C96" t="s">
-        <v>213</v>
+        <v>252</v>
       </c>
       <c r="D96" t="s">
         <v>100</v>
       </c>
       <c r="E96" t="s">
-        <v>214</v>
+        <v>213</v>
+      </c>
+      <c r="F96" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2344,7 +2373,7 @@
         <v>101</v>
       </c>
       <c r="E97" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -2352,203 +2381,216 @@
         <v>102</v>
       </c>
       <c r="E98" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D99" t="s">
-        <v>218</v>
+        <v>256</v>
       </c>
       <c r="E99" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D100" t="s">
-        <v>219</v>
+        <v>257</v>
       </c>
       <c r="E100" t="s">
-        <v>220</v>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D101" t="s">
+        <v>258</v>
+      </c>
+      <c r="E101" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A102">
-        <v>7</v>
-      </c>
-      <c r="B102" t="s">
-        <v>99</v>
-      </c>
-      <c r="C102" t="s">
-        <v>223</v>
-      </c>
       <c r="D102" t="s">
-        <v>203</v>
-      </c>
-      <c r="E102" t="s">
-        <v>224</v>
-      </c>
-      <c r="F102" t="s">
-        <v>225</v>
+        <v>259</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B104" t="s">
         <v>99</v>
       </c>
       <c r="C104" t="s">
-        <v>246</v>
+        <v>219</v>
       </c>
       <c r="D104" t="s">
         <v>203</v>
       </c>
       <c r="E104" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D105" t="s">
-        <v>238</v>
-      </c>
-      <c r="E105" t="s">
-        <v>248</v>
+        <v>220</v>
+      </c>
+      <c r="F104" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>8</v>
+      </c>
+      <c r="B106" t="s">
+        <v>99</v>
+      </c>
+      <c r="C106" t="s">
+        <v>242</v>
+      </c>
       <c r="D106" t="s">
-        <v>239</v>
+        <v>203</v>
       </c>
       <c r="E106" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D107" t="s">
+        <v>234</v>
+      </c>
       <c r="E107" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D108" t="s">
+        <v>235</v>
+      </c>
       <c r="E108" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E109" t="s">
-        <v>240</v>
+        <v>246</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E110" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A111">
+      <c r="E111" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113">
         <v>9</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B113" t="s">
         <v>99</v>
       </c>
-      <c r="C111" t="s">
-        <v>229</v>
-      </c>
-      <c r="D111" t="s">
+      <c r="C113" t="s">
+        <v>225</v>
+      </c>
+      <c r="D113" t="s">
         <v>211</v>
       </c>
-      <c r="E111" t="s">
-        <v>232</v>
-      </c>
-      <c r="F111" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D112" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D113" t="s">
+      <c r="E113" t="s">
+        <v>228</v>
+      </c>
+      <c r="F113" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D114" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D115" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D114" t="s">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D116" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D115" t="s">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D117" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D116" t="s">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D118" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A118">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120">
         <v>10</v>
-      </c>
-      <c r="B118" t="s">
-        <v>99</v>
-      </c>
-      <c r="C118" t="s">
-        <v>226</v>
-      </c>
-      <c r="D118" t="s">
-        <v>227</v>
-      </c>
-      <c r="E118" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A120">
-        <v>11</v>
       </c>
       <c r="B120" t="s">
         <v>99</v>
       </c>
       <c r="C120" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D120" t="s">
+        <v>223</v>
+      </c>
+      <c r="E120" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>11</v>
+      </c>
+      <c r="B122" t="s">
+        <v>99</v>
+      </c>
+      <c r="C122" t="s">
+        <v>217</v>
+      </c>
+      <c r="D122" t="s">
         <v>132</v>
       </c>
-      <c r="E120" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D121" t="s">
+      <c r="E122" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D123" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D122" t="s">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D124" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D123" t="s">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D125" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A125">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A127">
         <v>12</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B127" t="s">
         <v>99</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C127" t="s">
         <v>200</v>
       </c>
-      <c r="D125" t="s">
+      <c r="D127" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D126" t="s">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D128" t="s">
         <v>202</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor updates to results scripts
</commit_message>
<xml_diff>
--- a/script_overview.xlsx
+++ b/script_overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Documents\projects\Yale\resstock_projections\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pb637\Documents\projects\Yale\resstock_projections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917130FD-8833-47A2-B185-4F7EAAF5DC38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E060B5D-5D06-4AA3-A3DC-02728C676184}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1073" yWindow="1073" windowWidth="14400" windowHeight="7372" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="projection" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="261">
   <si>
     <t>Folder</t>
   </si>
@@ -814,6 +814,9 @@
   </si>
   <si>
     <t>ExtData/CapExIns.csv</t>
+  </si>
+  <si>
+    <t>similar as hiDR for all hiMF outputs, e.g. rs_hiMF_EG.RData, etc.</t>
   </si>
 </sst>
 </file>
@@ -1134,17 +1137,17 @@
   <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1164,7 +1167,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1181,7 +1184,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D3" t="s">
         <v>19</v>
       </c>
@@ -1189,7 +1192,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D4" t="s">
         <v>20</v>
       </c>
@@ -1197,12 +1200,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1219,7 +1222,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D7" t="s">
         <v>19</v>
       </c>
@@ -1227,7 +1230,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D8" t="s">
         <v>20</v>
       </c>
@@ -1235,12 +1238,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1257,7 +1260,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D11" t="s">
         <v>19</v>
       </c>
@@ -1265,7 +1268,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D12" t="s">
         <v>20</v>
       </c>
@@ -1273,12 +1276,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>4</v>
       </c>
@@ -1298,7 +1301,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D15" t="s">
         <v>8</v>
       </c>
@@ -1306,7 +1309,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D16" t="s">
         <v>9</v>
       </c>
@@ -1314,7 +1317,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>5</v>
       </c>
@@ -1334,7 +1337,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D18" t="s">
         <v>32</v>
       </c>
@@ -1342,7 +1345,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D19" t="s">
         <v>33</v>
       </c>
@@ -1350,7 +1353,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D20" t="s">
         <v>34</v>
       </c>
@@ -1358,22 +1361,22 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>6</v>
       </c>
@@ -1393,7 +1396,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D25" t="s">
         <v>32</v>
       </c>
@@ -1401,12 +1404,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E26" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>7</v>
       </c>
@@ -1426,22 +1429,22 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E28" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E29" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E30" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>8</v>
       </c>
@@ -1461,7 +1464,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>9</v>
       </c>
@@ -1481,12 +1484,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D33" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>10</v>
       </c>
@@ -1503,7 +1506,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D35" t="s">
         <v>60</v>
       </c>
@@ -1511,12 +1514,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D36" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>11</v>
       </c>
@@ -1536,7 +1539,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D38" t="s">
         <v>67</v>
       </c>
@@ -1544,7 +1547,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D39" t="s">
         <v>68</v>
       </c>
@@ -1552,37 +1555,37 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D40" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D41" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D42" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D43" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D44" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D45" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>12</v>
       </c>
@@ -1602,7 +1605,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>13</v>
       </c>
@@ -1622,27 +1625,27 @@
         <v>82</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D48" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D49" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D50" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D51" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>14</v>
       </c>
@@ -1662,7 +1665,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D53" t="s">
         <v>92</v>
       </c>
@@ -1670,7 +1673,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D54" t="s">
         <v>93</v>
       </c>
@@ -1678,12 +1681,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D55" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D56" t="s">
         <v>95</v>
       </c>
@@ -1695,21 +1698,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B77A6A4-E700-4667-BE58-A58B09F8FC11}">
-  <dimension ref="A1:F128"/>
+  <dimension ref="A1:F129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.109375" customWidth="1"/>
-    <col min="5" max="5" width="43.5546875" customWidth="1"/>
+    <col min="4" max="4" width="50.1328125" customWidth="1"/>
+    <col min="5" max="5" width="43.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1729,7 +1732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1749,7 +1752,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D3" t="s">
         <v>172</v>
       </c>
@@ -1757,7 +1760,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D4" t="s">
         <v>173</v>
       </c>
@@ -1765,7 +1768,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D5" t="s">
         <v>174</v>
       </c>
@@ -1773,7 +1776,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D6" t="s">
         <v>175</v>
       </c>
@@ -1781,7 +1784,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D7" t="s">
         <v>176</v>
       </c>
@@ -1789,7 +1792,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D8" t="s">
         <v>177</v>
       </c>
@@ -1797,7 +1800,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D9" t="s">
         <v>178</v>
       </c>
@@ -1805,7 +1808,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D10" t="s">
         <v>179</v>
       </c>
@@ -1813,107 +1816,107 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D11" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D13" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D14" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D15" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D16" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D17" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D18" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D19" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D20" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D21" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D22" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D23" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D24" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D25" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D26" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D27" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D28" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D29" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D30" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>2</v>
       </c>
@@ -1933,7 +1936,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D33" t="s">
         <v>101</v>
       </c>
@@ -1941,7 +1944,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D34" t="s">
         <v>102</v>
       </c>
@@ -1949,32 +1952,32 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E35" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E36" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E37" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E38" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E39" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>3</v>
       </c>
@@ -1994,7 +1997,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D42" t="s">
         <v>66</v>
       </c>
@@ -2002,22 +2005,22 @@
         <v>164</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D43" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D44" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D45" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>4</v>
       </c>
@@ -2037,7 +2040,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D48" t="s">
         <v>113</v>
       </c>
@@ -2045,7 +2048,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D49" t="s">
         <v>114</v>
       </c>
@@ -2053,7 +2056,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="50" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D50" t="s">
         <v>115</v>
       </c>
@@ -2061,7 +2064,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D51" t="s">
         <v>116</v>
       </c>
@@ -2069,7 +2072,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="52" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D52" t="s">
         <v>117</v>
       </c>
@@ -2077,7 +2080,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="53" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D53" t="s">
         <v>118</v>
       </c>
@@ -2085,7 +2088,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="54" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D54" t="s">
         <v>119</v>
       </c>
@@ -2093,7 +2096,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="55" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D55" t="s">
         <v>100</v>
       </c>
@@ -2101,7 +2104,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="56" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D56" t="s">
         <v>101</v>
       </c>
@@ -2109,7 +2112,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="57" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D57" t="s">
         <v>102</v>
       </c>
@@ -2117,7 +2120,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="58" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D58" t="s">
         <v>120</v>
       </c>
@@ -2125,7 +2128,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="59" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D59" t="s">
         <v>121</v>
       </c>
@@ -2133,7 +2136,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="60" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D60" t="s">
         <v>122</v>
       </c>
@@ -2141,7 +2144,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="61" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D61" t="s">
         <v>123</v>
       </c>
@@ -2149,7 +2152,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="62" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D62" t="s">
         <v>124</v>
       </c>
@@ -2157,7 +2160,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="63" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D63" t="s">
         <v>125</v>
       </c>
@@ -2165,7 +2168,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="64" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D64" t="s">
         <v>126</v>
       </c>
@@ -2173,7 +2176,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D65" t="s">
         <v>127</v>
       </c>
@@ -2181,7 +2184,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D66" t="s">
         <v>128</v>
       </c>
@@ -2189,7 +2192,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D67" t="s">
         <v>129</v>
       </c>
@@ -2197,7 +2200,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D68" t="s">
         <v>130</v>
       </c>
@@ -2205,392 +2208,397 @@
         <v>153</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:5" x14ac:dyDescent="0.45">
       <c r="E69" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="4:5" x14ac:dyDescent="0.45">
       <c r="E70" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="4:5" x14ac:dyDescent="0.45">
       <c r="E71" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="4:5" x14ac:dyDescent="0.45">
       <c r="E72" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="4:5" x14ac:dyDescent="0.45">
       <c r="E73" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="4:5" x14ac:dyDescent="0.45">
       <c r="E74" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="4:5" x14ac:dyDescent="0.45">
       <c r="E75" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="4:5" x14ac:dyDescent="0.45">
       <c r="E76" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="4:5" x14ac:dyDescent="0.45">
       <c r="E77" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="4:5" x14ac:dyDescent="0.45">
       <c r="E78" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80">
+    <row r="79" spans="4:5" x14ac:dyDescent="0.45">
+      <c r="E79" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A81">
         <v>5</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B81" t="s">
         <v>99</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C81" t="s">
         <v>241</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D81" t="s">
         <v>203</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E81" t="s">
         <v>211</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F81" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D81" t="s">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D82" t="s">
         <v>204</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E82" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D82" t="s">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D83" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D83" t="s">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D84" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D84" t="s">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D85" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D85" t="s">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D86" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D86" t="s">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D87" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D87" t="s">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D88" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D88" t="s">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D89" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D89" t="s">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D90" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D90" t="s">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D91" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D91" t="s">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D92" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D92" t="s">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D93" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D93" t="s">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D94" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D94" t="s">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D95" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A97">
         <v>6</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B97" t="s">
         <v>99</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C97" t="s">
         <v>252</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D97" t="s">
         <v>100</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E97" t="s">
         <v>213</v>
       </c>
-      <c r="F96" t="s">
+      <c r="F97" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D97" t="s">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D98" t="s">
         <v>101</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E98" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D98" t="s">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D99" t="s">
         <v>102</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E99" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D99" t="s">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D100" t="s">
         <v>256</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E100" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D100" t="s">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D101" t="s">
         <v>257</v>
       </c>
-      <c r="E100" t="s">
+      <c r="E101" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D101" t="s">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D102" t="s">
         <v>258</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E102" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D102" t="s">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D103" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A104">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A105">
         <v>7</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B105" t="s">
         <v>99</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C105" t="s">
         <v>219</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D105" t="s">
         <v>203</v>
       </c>
-      <c r="E104" t="s">
+      <c r="E105" t="s">
         <v>220</v>
       </c>
-      <c r="F104" t="s">
+      <c r="F105" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A106">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A107">
         <v>8</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B107" t="s">
         <v>99</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C107" t="s">
         <v>242</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D107" t="s">
         <v>203</v>
       </c>
-      <c r="E106" t="s">
+      <c r="E107" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D107" t="s">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D108" t="s">
         <v>234</v>
       </c>
-      <c r="E107" t="s">
+      <c r="E108" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D108" t="s">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D109" t="s">
         <v>235</v>
       </c>
-      <c r="E108" t="s">
+      <c r="E109" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E109" t="s">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E110" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E110" t="s">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E111" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E111" t="s">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E112" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A113">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A114">
         <v>9</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B114" t="s">
         <v>99</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C114" t="s">
         <v>225</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D114" t="s">
         <v>211</v>
       </c>
-      <c r="E113" t="s">
+      <c r="E114" t="s">
         <v>228</v>
       </c>
-      <c r="F113" t="s">
+      <c r="F114" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D114" t="s">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D115" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D115" t="s">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D116" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D116" t="s">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D117" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D117" t="s">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D118" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D118" t="s">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D119" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A120">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A121">
         <v>10</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B121" t="s">
         <v>99</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C121" t="s">
         <v>222</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D121" t="s">
         <v>223</v>
       </c>
-      <c r="E120" t="s">
+      <c r="E121" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A122">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A123">
         <v>11</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B123" t="s">
         <v>99</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C123" t="s">
         <v>217</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D123" t="s">
         <v>132</v>
       </c>
-      <c r="E122" t="s">
+      <c r="E123" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D123" t="s">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D124" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D124" t="s">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D125" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D125" t="s">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D126" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A127">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A128">
         <v>12</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B128" t="s">
         <v>99</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C128" t="s">
         <v>200</v>
       </c>
-      <c r="D127" t="s">
+      <c r="D128" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D128" t="s">
+    <row r="129" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D129" t="s">
         <v>202</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add figures data, add Info to script_overview
</commit_message>
<xml_diff>
--- a/script_overview.xlsx
+++ b/script_overview.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pb637\Documents\projects\Yale\resstock_projections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E060B5D-5D06-4AA3-A3DC-02728C676184}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727F11CA-5FE4-4A9C-A22C-D5A27FB49B10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1073" yWindow="1073" windowWidth="14400" windowHeight="7372" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="projection" sheetId="1" r:id="rId1"/>
     <sheet name="results" sheetId="3" r:id="rId2"/>
+    <sheet name="Info" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="293">
   <si>
     <t>Folder</t>
   </si>
@@ -219,9 +220,6 @@
     <t>All the corresponding HP_redo files in Eagle_outputs/HP_redo/</t>
   </si>
   <si>
-    <t>Combine all of the succesful original simulations with all the files which had to be redone due to faulty HVAC/HP combinations (redone in HP_redo) and save in resstock results .RData files in Eagle_outputs/Complete_results. Also replace a few residual unexplained failed simulations with versions of the same building from subequent simulation years</t>
-  </si>
-  <si>
     <t>The *_final.RData res files in Eagle_outputs/Complete_results, including all corrections and resolved/replaced failed simulations.</t>
   </si>
   <si>
@@ -639,12 +637,6 @@
     <t>RECS_checks</t>
   </si>
   <si>
-    <t>Yale Courses/Research/RECS research/RECS2015/recs2015_public_v4.csv</t>
-  </si>
-  <si>
-    <t>Yale Courses/Research/RECS research/RECS2009/recs2009_public.csv</t>
-  </si>
-  <si>
     <t>ExtData/US_FA_GHG_summaries.RData</t>
   </si>
   <si>
@@ -783,9 +775,6 @@
     <t>County_Scenario_SM_Results.Rdata. For access email peter.berrill@aya.yale.edu</t>
   </si>
   <si>
-    <t>All of the future construction files for each housing stock/new housing characteristics scenario in scen_bscsv. For access email peter.berrill@aya.yale.edu</t>
-  </si>
-  <si>
     <t>Calculate % reductions in final energy consumption from different renovation families in each renovation scenario, for SI Tables S6 and S7. Calculate number of renovations by type in each ren scenario</t>
   </si>
   <si>
@@ -817,19 +806,637 @@
   </si>
   <si>
     <t>similar as hiDR for all hiMF outputs, e.g. rs_hiMF_EG.RData, etc.</t>
+  </si>
+  <si>
+    <t>All of the future construction files for each housing stock/new housing characteristics scenario in scen_bscsv. For access see LF Data repository</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most data files that are not available on the archived github repository for this publication are large data files which are available on the accompanying Zenodo Large File repository. </t>
+  </si>
+  <si>
+    <t>Some redundant data are not available either on the archived github repository or the Zenodo Large File repository.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For instance, results csv files from the ResStock simulation are unavailable, as they are available already in combined/cleaned form in the `Eagle_outputs/Complete_results` and `Final_results` folders of the LF Zenodo data repository. </t>
+  </si>
+  <si>
+    <t>For access to the results csv files please contact peter.berrill@aya.yale.edu</t>
+  </si>
+  <si>
+    <t>June 15 2022</t>
+  </si>
+  <si>
+    <t>The execution of the files should be as follows:</t>
+  </si>
+  <si>
+    <t>Combine all of the succesful original simulations with all the files which had to be redone due to faulty HVAC/HP combinations (redone in HP_redo) and save in resstock results .RData files in Eagle_outputs/Complete_results/. Also replace a few residual unexplained failed simulations with versions of the same building from subequent simulation years</t>
+  </si>
+  <si>
+    <t>projection scripts:</t>
+  </si>
+  <si>
+    <r>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>decay.R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>renScenariosReg.R, renScenariosAdv.R, renScenariosExEl.R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>create_bscsv_sim.R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HSMtoResStock.R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>5.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bs_adjust.R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>6.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bs_adjust_incompatible_combos.R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>7.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bs_adjust_HP.R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>8.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HP_fail_replace.R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>9.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rs_fail_replace.R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CharacteristicsNewHousing.R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>11.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>weights_NC.R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>12.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GHGint.R</t>
+    </r>
+  </si>
+  <si>
+    <t>results_scripts:</t>
+  </si>
+  <si>
+    <r>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RS_results_ren.R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RS_results_ren_assess.R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ren_GHG.R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RS_results_proj</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>5.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ren_ass_stock</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>6.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ren_assess_strategy</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>7.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tot_GHG_2005_2020.R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>8.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RS_results_all</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>9.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>map_results_strategies.R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>land_use.R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>11.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>develop_newHP</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>12.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RECS_checks</t>
+    </r>
+  </si>
+  <si>
+    <t>recs2009_public.csv (access here https://www.eia.gov/consumption/residential/)</t>
+  </si>
+  <si>
+    <t>recs2015_public_v4.csv (access here https://www.eia.gov/consumption/residential/)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -852,8 +1459,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1137,8 +1750,8 @@
   <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1387,7 +2000,7 @@
         <v>39</v>
       </c>
       <c r="D24" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E24" t="s">
         <v>41</v>
@@ -1420,7 +2033,7 @@
         <v>43</v>
       </c>
       <c r="D27" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="E27" t="s">
         <v>45</v>
@@ -1455,10 +2068,10 @@
         <v>49</v>
       </c>
       <c r="D31" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E31" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F31" t="s">
         <v>50</v>
@@ -1503,7 +2116,7 @@
         <v>59</v>
       </c>
       <c r="F34" t="s">
-        <v>61</v>
+        <v>264</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
@@ -1511,12 +2124,12 @@
         <v>60</v>
       </c>
       <c r="E35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
@@ -1527,62 +2140,62 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D38" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
@@ -1593,16 +2206,16 @@
         <v>5</v>
       </c>
       <c r="C46" t="s">
+        <v>77</v>
+      </c>
+      <c r="D46" t="s">
         <v>78</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>79</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>80</v>
-      </c>
-      <c r="F46" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
@@ -1613,26 +2226,26 @@
         <v>5</v>
       </c>
       <c r="C47" t="s">
+        <v>82</v>
+      </c>
+      <c r="D47" t="s">
         <v>83</v>
       </c>
-      <c r="D47" t="s">
-        <v>84</v>
-      </c>
       <c r="E47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
@@ -1642,7 +2255,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D51" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
@@ -1653,42 +2266,42 @@
         <v>5</v>
       </c>
       <c r="C52" t="s">
+        <v>88</v>
+      </c>
+      <c r="D52" t="s">
+        <v>90</v>
+      </c>
+      <c r="E52" t="s">
+        <v>95</v>
+      </c>
+      <c r="F52" t="s">
         <v>89</v>
-      </c>
-      <c r="D52" t="s">
-        <v>91</v>
-      </c>
-      <c r="E52" t="s">
-        <v>96</v>
-      </c>
-      <c r="F52" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E53" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E54" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D55" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1701,8 +2314,8 @@
   <dimension ref="A1:F129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E99" sqref="E99"/>
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D129" sqref="D129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1737,183 +2350,183 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D24" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D26" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
@@ -1921,60 +2534,60 @@
         <v>2</v>
       </c>
       <c r="B32" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" t="s">
+        <v>235</v>
+      </c>
+      <c r="D32" t="s">
         <v>99</v>
       </c>
-      <c r="C32" t="s">
-        <v>238</v>
-      </c>
-      <c r="D32" t="s">
-        <v>100</v>
-      </c>
       <c r="E32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F32" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E35" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E36" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E37" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E38" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
@@ -1982,42 +2595,42 @@
         <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C41" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E41" t="s">
+        <v>106</v>
+      </c>
+      <c r="F41" t="s">
         <v>107</v>
-      </c>
-      <c r="F41" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D45" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
@@ -2025,242 +2638,242 @@
         <v>4</v>
       </c>
       <c r="B47" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C47" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D47" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E47" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F47" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="49" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D49" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E49" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E50" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="51" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D51" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E51" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D52" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E52" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D53" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E53" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D54" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E54" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D55" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E55" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E56" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="57" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D57" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E57" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D58" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="59" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D59" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E59" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="60" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D60" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E60" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="61" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D61" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E61" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="62" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D62" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E62" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="63" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D63" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E63" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="64" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D64" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E64" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="65" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D65" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E65" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="66" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D66" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E66" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="67" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D67" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E67" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="68" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D68" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E68" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="69" spans="4:5" x14ac:dyDescent="0.45">
       <c r="E69" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="70" spans="4:5" x14ac:dyDescent="0.45">
       <c r="E70" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="71" spans="4:5" x14ac:dyDescent="0.45">
       <c r="E71" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="72" spans="4:5" x14ac:dyDescent="0.45">
       <c r="E72" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="73" spans="4:5" x14ac:dyDescent="0.45">
       <c r="E73" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="74" spans="4:5" x14ac:dyDescent="0.45">
       <c r="E74" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="75" spans="4:5" x14ac:dyDescent="0.45">
       <c r="E75" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="76" spans="4:5" x14ac:dyDescent="0.45">
       <c r="E76" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="77" spans="4:5" x14ac:dyDescent="0.45">
       <c r="E77" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="78" spans="4:5" x14ac:dyDescent="0.45">
       <c r="E78" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="79" spans="4:5" x14ac:dyDescent="0.45">
       <c r="E79" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.45">
@@ -2268,92 +2881,92 @@
         <v>5</v>
       </c>
       <c r="B81" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C81" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D81" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E81" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F81" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D82" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E82" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D83" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D84" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D85" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D86" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D87" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D88" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D89" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D90" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D91" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D92" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D93" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D94" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D95" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.45">
@@ -2361,64 +2974,64 @@
         <v>6</v>
       </c>
       <c r="B97" t="s">
+        <v>98</v>
+      </c>
+      <c r="C97" t="s">
+        <v>248</v>
+      </c>
+      <c r="D97" t="s">
         <v>99</v>
       </c>
-      <c r="C97" t="s">
-        <v>252</v>
-      </c>
-      <c r="D97" t="s">
-        <v>100</v>
-      </c>
       <c r="E97" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F97" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D98" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E98" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D99" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E99" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D100" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E100" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D101" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E101" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D102" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E102" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D103" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.45">
@@ -2426,19 +3039,19 @@
         <v>7</v>
       </c>
       <c r="B105" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C105" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D105" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E105" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F105" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.45">
@@ -2446,47 +3059,47 @@
         <v>8</v>
       </c>
       <c r="B107" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C107" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D107" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E107" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D108" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E108" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D109" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E109" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E110" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E111" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E112" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.45">
@@ -2494,44 +3107,44 @@
         <v>9</v>
       </c>
       <c r="B114" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C114" t="s">
+        <v>222</v>
+      </c>
+      <c r="D114" t="s">
+        <v>208</v>
+      </c>
+      <c r="E114" t="s">
         <v>225</v>
       </c>
-      <c r="D114" t="s">
-        <v>211</v>
-      </c>
-      <c r="E114" t="s">
-        <v>228</v>
-      </c>
       <c r="F114" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D115" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D116" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D117" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D118" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D119" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.45">
@@ -2539,16 +3152,16 @@
         <v>10</v>
       </c>
       <c r="B121" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C121" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D121" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E121" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.45">
@@ -2556,31 +3169,31 @@
         <v>11</v>
       </c>
       <c r="B123" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C123" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D123" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E123" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D124" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D125" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D126" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.45">
@@ -2588,21 +3201,198 @@
         <v>12</v>
       </c>
       <c r="B128" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C128" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D128" t="s">
-        <v>201</v>
+        <v>292</v>
       </c>
     </row>
     <row r="129" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D129" t="s">
-        <v>202</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{579FC3A7-FA10-4219-A895-AC3ADC2DF739}">
+  <dimension ref="A1:B35"/>
+  <sheetViews>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A23" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>